<commit_message>
Modified Install Instructions to note that all users with access to DL_Diag will have access to the tool.
</commit_message>
<xml_diff>
--- a/Permission List.xlsx
+++ b/Permission List.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Query To Get Exisiting Names" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CAPABILITYDB!$B$1:$C$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CAPABILITYDB!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="237">
   <si>
     <t>WWID</t>
   </si>
@@ -726,6 +726,9 @@
   </si>
   <si>
     <t xml:space="preserve">  WHERE [name] Like 'CED\%'</t>
+  </si>
+  <si>
+    <t>Prefix</t>
   </si>
 </sst>
 </file>
@@ -1081,6 +1084,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2371,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C91"/>
+  <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>